<commit_message>
Code runt nu eindelijk in py
</commit_message>
<xml_diff>
--- a/Bus Planning Casus 1.xlsx
+++ b/Bus Planning Casus 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/714af6a2766708e6/Python/PJ5ProjectGroep4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_0399E22E9067360E62355476585DCE3A87431D38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A5F0255-45B4-414D-A51F-7403B93893E1}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_0399E22E9067360E62355476585DCE3A87431D38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEEF2AFD-FB34-43B8-BD71-FEEF9019C142}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,9 +155,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -176,7 +174,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -187,6 +229,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{048CA90A-A8CD-4B6B-A6FB-578AB318751B}" name="Table1" displayName="Table1" ref="A1:H12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:H12" xr:uid="{048CA90A-A8CD-4B6B-A6FB-578AB318751B}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{27F0D1C4-D99B-48D9-A6B0-9F960B51B487}" name="start location"/>
+    <tableColumn id="2" xr3:uid="{82A99C57-134F-42D8-8B89-A78957CB7ABD}" name="end location"/>
+    <tableColumn id="3" xr3:uid="{DCD852A7-B047-4A0E-A087-6DDEC9B2C6E4}" name="start time"/>
+    <tableColumn id="4" xr3:uid="{6CBF6260-379F-4C62-9FDE-57C24C3A7F8E}" name="end time"/>
+    <tableColumn id="5" xr3:uid="{B899A05F-D45F-4B70-B0BB-E6832DC7C552}" name="activity"/>
+    <tableColumn id="6" xr3:uid="{498C8757-E9FC-4E00-98C5-D6240767D58C}" name="line"/>
+    <tableColumn id="7" xr3:uid="{BC2B4D10-B7E2-4BD2-96C9-C54298FFD29A}" name="energy consumption"/>
+    <tableColumn id="8" xr3:uid="{0B058C4D-109B-4FA1-BF35-B9232D289732}" name="bus"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -477,14 +536,17 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -783,6 +845,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -796,6 +861,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="85" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="f20b580f4bc73672f7fc26b54f2fdd7d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9324efb3ca4fd789e46a4cfe415928a3" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -1016,14 +1089,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C58A68F-A5E9-4F6F-AD01-06B5D5C01F66}">
   <ds:schemaRefs>
@@ -1033,6 +1098,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABD986A7-2A39-40F9-A024-B808D196BF4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C21D0A-65D6-47B6-8E76-5D8CAE45D404}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1049,14 +1124,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABD986A7-2A39-40F9-A024-B808D196BF4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>